<commit_message>
plots per itarations in there
</commit_message>
<xml_diff>
--- a/data/LCOE_Parameters.xlsb.xlsx
+++ b/data/LCOE_Parameters.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanko\Desktop\personal\coding\OPV_SBSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6AC944-5010-4D18-823D-CA8BD7F91FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32311F31-6451-43C4-9070-60F2C18F483A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -1115,9 +1115,6 @@
     <xf numFmtId="165" fontId="0" fillId="17" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="19" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1126,6 +1123,9 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6194,8 +6194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE2CF3A-0F0C-4B1F-85F5-0856EF79378A}">
   <dimension ref="A2:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8704,7 +8704,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
       <c r="P11" s="30"/>
-      <c r="Q11" s="65">
+      <c r="Q11" s="64">
         <f>IF(Q29="PV",0.096,IF(Q29="OPV",0.016,"Choose Technology"))</f>
         <v>1.6E-2</v>
       </c>
@@ -8904,7 +8904,7 @@
       </c>
       <c r="K16" s="30"/>
       <c r="L16" s="30"/>
-      <c r="M16" s="64">
+      <c r="M16" s="63">
         <f>(IF(Q29="PV",0.2,IF(Q29="OPV",0.35,"Choose Technology")))*Table14232425[[#This Row],[Mean]]</f>
         <v>4.725E-3</v>
       </c>
@@ -8954,7 +8954,7 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
       <c r="P17" s="30"/>
-      <c r="Q17" s="63">
+      <c r="Q17" s="62">
         <v>0.06</v>
       </c>
       <c r="R17" s="48"/>
@@ -11964,10 +11964,10 @@
       <c r="B2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="62"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
fixing error with get_cost because it returned a referene instead of a copy. it returns a copy now
</commit_message>
<xml_diff>
--- a/data/LCOE_Parameters.xlsb.xlsx
+++ b/data/LCOE_Parameters.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanko\Desktop\personal\coding\OPV_SBSP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32311F31-6451-43C4-9070-60F2C18F483A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDF0BB6-0A59-4AD3-A3CC-1725579C7864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="3" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5EE87DF2-9FC5-4DDF-A454-2AABC6FB7A6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="152">
   <si>
     <t>LCOE</t>
   </si>
@@ -4130,7 +4130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1BE8353-515E-4AA9-9C02-80594D610788}">
   <dimension ref="A2:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -6194,8 +6194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE2CF3A-0F0C-4B1F-85F5-0856EF79378A}">
   <dimension ref="A2:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6862,9 +6862,6 @@
       </c>
       <c r="I21" t="s">
         <v>106</v>
-      </c>
-      <c r="J21" t="s">
-        <v>32</v>
       </c>
       <c r="Q21">
         <v>20</v>

</xml_diff>